<commit_message>
Alterações em diversas classes
</commit_message>
<xml_diff>
--- a/data/Geicom/importacaoMetasExport.xlsx
+++ b/data/Geicom/importacaoMetasExport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17595" windowHeight="6465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
   <si>
     <t>Indicador</t>
   </si>
@@ -36,7 +36,7 @@
     <t>01/01/2016 a 31/01/2016</t>
   </si>
   <si>
-    <t>Dias com manutenção da equipe mínima da Central de Regulação do SAMU</t>
+    <t>Taxa de Adesao Oficial</t>
   </si>
   <si>
     <t>310150</t>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>17.707.274/0001-18</t>
+  </si>
+  <si>
+    <t>Taxa de Adesao</t>
   </si>
   <si>
     <t>310420</t>
@@ -460,13 +463,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -504,16 +510,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>90</v>
@@ -524,13 +530,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
       </c>
       <c r="E4">
         <v>90</v>
@@ -538,16 +544,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>90</v>
@@ -558,13 +564,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>90</v>
@@ -572,16 +578,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>90</v>
@@ -592,13 +598,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>90</v>
@@ -606,18 +612,154 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="E9">
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17">
         <v>90</v>
       </c>
     </row>

</xml_diff>